<commit_message>
1. Solve the transaction problems. 2. Solve the database laking auto-increment. 3. Optmize the coding rule.
</commit_message>
<xml_diff>
--- a/Design/ocms_database_design_draft.xlsx
+++ b/Design/ocms_database_design_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6980" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16660" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="4" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>外部キー</t>
   </si>
   <si>
-    <t>items_checkitems_id</t>
-  </si>
-  <si>
     <t>チェックリスト名</t>
   </si>
   <si>
@@ -341,67 +338,15 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>、引用表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>checklist</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>、外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>名</t>
-    </r>
+      <t>外部キー、引用表item、外部キー名fk_item_checklists_item、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -411,8 +356,13 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_items_checklist</t>
-    </r>
+      <t>外部キー、引用表checkitem_status、外部キー名fk_item_checklists_checkitem_status、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <t>checkitem_id</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -420,7 +370,25 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
+      <t>外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、引用表</t>
     </r>
     <r>
       <rPr>
@@ -431,7 +399,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>not null</t>
+      <t>project</t>
     </r>
     <r>
       <rPr>
@@ -440,7 +408,25 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名</t>
     </r>
     <r>
       <rPr>
@@ -451,8 +437,20 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unsigned</t>
-    </r>
+      <t>fk_checklist_project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>。not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -460,7 +458,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>。外部キ</t>
+      <t>外部キ</t>
     </r>
     <r>
       <rPr>
@@ -478,7 +476,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>制限</t>
+      <t>、引用表</t>
     </r>
     <r>
       <rPr>
@@ -489,10 +487,8 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">On update cascade, On delete cascase </t>
-    </r>
-  </si>
-  <si>
+      <t>checklist</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -500,7 +496,25 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>引用表</t>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名</t>
     </r>
     <r>
       <rPr>
@@ -511,7 +525,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>item</t>
+      <t>fk_item_checklist</t>
     </r>
     <r>
       <rPr>
@@ -520,7 +534,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、参照列</t>
+      <t>、</t>
     </r>
     <r>
       <rPr>
@@ -531,7 +545,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>item_id</t>
+      <t>not null</t>
     </r>
     <r>
       <rPr>
@@ -540,25 +554,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>名：</t>
+      <t>、</t>
     </r>
     <r>
       <rPr>
@@ -569,7 +565,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_items_item</t>
+      <t>unsigned</t>
     </r>
     <r>
       <rPr>
@@ -578,7 +574,25 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
     </r>
     <r>
       <rPr>
@@ -589,8 +603,10 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>not null</t>
-    </r>
+      <t xml:space="preserve">On update cascade, On delete cascase </t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -598,7 +614,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
+      <t>引用表</t>
     </r>
     <r>
       <rPr>
@@ -609,7 +625,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unsigned</t>
+      <t>item</t>
     </r>
     <r>
       <rPr>
@@ -618,25 +634,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>。外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>制限</t>
+      <t>、参照列</t>
     </r>
     <r>
       <rPr>
@@ -647,10 +645,8 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
+      <t>item_id</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -658,7 +654,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>外部キ</t>
+      <t>、外部キ</t>
     </r>
     <r>
       <rPr>
@@ -676,7 +672,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、引用表</t>
+      <t>名：</t>
     </r>
     <r>
       <rPr>
@@ -687,7 +683,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>project</t>
+      <t>fk_item_item</t>
     </r>
     <r>
       <rPr>
@@ -696,25 +692,7 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>名</t>
+      <t>、</t>
     </r>
     <r>
       <rPr>
@@ -725,20 +703,17 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_checklists_project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>。not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
+      <t>not null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -748,10 +723,35 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表item、外部キー名fk_item_checklists_item、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
+      <t>unsigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -761,11 +761,11 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表checkitem_status、外部キー名fk_item_checklists_checkitem_status、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
-    <t>checkitem_id</t>
+      <t>On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <t>item_checkitem_status_id</t>
   </si>
   <si>
     <r>
@@ -777,7 +777,7 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表checkitem、外部キー名fk_chekitem_statuses_checkitem、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+      <t>外部キー、引用表checkitem、外部キー名fk_chekitem_status_checkitem、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
     </r>
   </si>
 </sst>
@@ -785,7 +785,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -831,14 +831,6 @@
       <color theme="1"/>
       <name val="Libian SC Regular"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -901,8 +893,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="325">
+  <cellStyleXfs count="345">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1922,7 +1974,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="325">
+  <cellStyles count="345">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2085,6 +2137,16 @@
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2247,6 +2309,16 @@
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2551,7 +2623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2590,7 +2662,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -2604,7 +2676,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -2618,7 +2690,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -2647,7 +2719,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2675,21 +2747,21 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -2703,19 +2775,19 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="57">
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
@@ -2753,7 +2825,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2783,7 +2855,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -2797,7 +2869,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -2811,7 +2883,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
@@ -2823,13 +2895,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="48">
@@ -2837,13 +2909,13 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2863,13 +2935,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="6"/>
     <col min="4" max="4" width="72.33203125" style="6" customWidth="1"/>
     <col min="5" max="16384" width="8.83203125" style="6"/>
@@ -2892,7 +2964,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -2906,13 +2978,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28">
@@ -2920,13 +2992,13 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2963,7 +3035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2993,7 +3065,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -3004,10 +3076,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
@@ -3016,22 +3088,22 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
@@ -3041,17 +3113,17 @@
     <row r="6" spans="1:4">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -3060,34 +3132,34 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>12</v>
@@ -3099,7 +3171,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -3125,7 +3197,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3154,7 +3226,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -3165,22 +3237,22 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -3189,10 +3261,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
update database design and work record
</commit_message>
<xml_diff>
--- a/Design/ocms_database_design_draft.xlsx
+++ b/Design/ocms_database_design_draft.xlsx
@@ -1,33 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuich\OneDrive\ドキュメント\Checklist\Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16660" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="4" r:id="rId1"/>
     <sheet name="checklist" sheetId="3" r:id="rId2"/>
     <sheet name="item" sheetId="2" r:id="rId3"/>
-    <sheet name="item_checkitem_status" sheetId="5" r:id="rId4"/>
-    <sheet name="checkitem_status" sheetId="6" r:id="rId5"/>
-    <sheet name="checkitem" sheetId="1" r:id="rId6"/>
+    <sheet name="checkitem_status" sheetId="6" r:id="rId4"/>
+    <sheet name="checkitem" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="79">
   <si>
     <t>カラム名</t>
     <rPh sb="3" eb="4">
@@ -62,10 +66,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>varchar(15)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>主キー、自動採番、not null、unsigned</t>
   </si>
   <si>
@@ -85,7 +85,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -97,9 +97,6 @@
     <t>not null</t>
   </si>
   <si>
-    <t>varchar(15)</t>
-  </si>
-  <si>
     <t>double</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>checkitem_status_id</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t>重要度</t>
   </si>
   <si>
-    <t>補充説明</t>
-  </si>
-  <si>
     <t>変更履歴</t>
   </si>
   <si>
@@ -220,10 +211,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>checkitem_id</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -232,10 +219,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>item_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>checklist_id</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -305,7 +288,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -325,7 +308,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -334,33 +317,95 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+    <t>checkitem_id</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、引用表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表item、外部キー名fk_item_checklists_item、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表checkitem_status、外部キー名fk_item_checklists_checkitem_status、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
-    <t>checkitem_id</t>
+      <t>fk_checklist_project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>。not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
   </si>
   <si>
     <r>
@@ -394,12 +439,12 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>project</t>
+      <t>checklist</t>
     </r>
     <r>
       <rPr>
@@ -432,25 +477,13 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_checklist_project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>。not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
+      <t>fk_item_checklist</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -458,36 +491,18 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>、引用表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>checklist</t>
+      <t>not null</t>
     </r>
     <r>
       <rPr>
@@ -496,36 +511,18 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_item_checklist</t>
+      <t>unsigned</t>
     </r>
     <r>
       <rPr>
@@ -534,19 +531,39 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>not null</t>
-    </r>
+      <t xml:space="preserve">On update cascade, On delete cascase </t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -554,18 +571,18 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>引用表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unsigned</t>
+      <t>item</t>
     </r>
     <r>
       <rPr>
@@ -574,39 +591,19 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>。外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>制限</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、参照列</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">On update cascade, On delete cascase </t>
-    </r>
-  </si>
-  <si>
+      <t>item_id</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -614,18 +611,36 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>引用表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>item</t>
+      <t>fk_item_item</t>
     </r>
     <r>
       <rPr>
@@ -634,18 +649,18 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、参照列</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>item_id</t>
+      <t>not null</t>
     </r>
     <r>
       <rPr>
@@ -654,36 +669,18 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>名：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_item_item</t>
+      <t>unsigned</t>
     </r>
     <r>
       <rPr>
@@ -692,111 +689,275 @@
         <rFont val="Libian SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>not null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unsigned</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>。外部キ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Lantinghei SC Demibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>ー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Libian SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t>制限</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+      <t>外部キー、引用表checkitem、外部キー名fk_chekitem_status_checkitem、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:NO 1:YES</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>補足説明</t>
+    <rPh sb="0" eb="2">
+      <t>ホソク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ガイド的な情報を付与</t>
+    <rPh sb="3" eb="4">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>フヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザが自由にコメント</t>
+    <rPh sb="4" eb="6">
+      <t>ジユウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロジェクトタイプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>詳細はのちに検討</t>
+    <rPh sb="0" eb="2">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ケントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>varchar(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>On update cascade, On delete cascade</t>
-    </r>
-  </si>
-  <si>
-    <t>item_checkitem_status_id</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表checkitem、外部キー名fk_chekitem_status_checkitem、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
-    </r>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>varchar(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>varchar(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コメントの根拠となる成果物</t>
+    <rPh sb="5" eb="7">
+      <t>コンキョ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>セイカブツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>典型的な成果物</t>
+    <rPh sb="0" eb="3">
+      <t>テンケイテキ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>セイカブツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varcher(200)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varcher(100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外部キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>item_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外部キー、引用表item、外部キー名fk_chekitem_status_item、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>typical_deliverables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>成果物の例</t>
+    <rPh sb="0" eb="3">
+      <t>セイカブツ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -805,7 +966,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -814,7 +975,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -837,6 +998,31 @@
       <color theme="1"/>
       <name val="Lantinghei SC Demibold"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1930,7 +2116,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1950,9 +2136,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -1973,353 +2156,368 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="345">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="344" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2377,7 +2575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2429,7 +2627,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2623,7 +2821,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2633,11 +2831,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
@@ -2662,27 +2860,27 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2690,13 +2888,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2719,10 +2917,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
@@ -2742,71 +2940,71 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="49">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="9"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2824,11 +3022,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -2852,70 +3050,70 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="54">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="48">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="48">
+        <v>10</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="54">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2932,114 +3130,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="12.83203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="6"/>
-    <col min="4" max="4" width="72.33203125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28">
-      <c r="A4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="14.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="17" style="6" customWidth="1"/>
@@ -3062,122 +3159,136 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" ht="28">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="36">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="36">
+      <c r="A11" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3192,15 +3303,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="14" style="6" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" style="6" customWidth="1"/>
@@ -3223,58 +3334,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" s="14" customFormat="1">
+      <c r="A6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>